<commit_message>
Updated PCB generated content
</commit_message>
<xml_diff>
--- a/altium_pcb/PCB_Project/Project Outputs for PCB_Project/Bill of Materials/Bill of Materials-PCB_Project.xlsx
+++ b/altium_pcb/PCB_Project/Project Outputs for PCB_Project/Bill of Materials/Bill of Materials-PCB_Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\continuum\eng\elec\y3s2\ee356\projects\ee356-project\ee356-project\altium_pcb\PCB_Project\Project Outputs for PCB_Project\Bill of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16B7E6A6-3982-496F-ACE7-21A4A45BCF57}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37BD2D70-337B-4FA9-B144-CBE558F6876D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List Report" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="133">
   <si>
     <t>Project Full Path</t>
   </si>
@@ -131,10 +131,10 @@
     <t>&lt;Parameter ClientContactEmail not found&gt;</t>
   </si>
   <si>
-    <t>08 Jan 2023</t>
-  </si>
-  <si>
-    <t>2158h</t>
+    <t>08 Feb 2023</t>
+  </si>
+  <si>
+    <t>1321h</t>
   </si>
   <si>
     <t>&lt;Parameter ClientWebsite not found&gt;</t>
@@ -293,7 +293,7 @@
     <t>General Type Carbon Film Resistor 2.2kOhm 1/4W 5% Axial Bulk</t>
   </si>
   <si>
-    <t>General Type Carbon Film Resistor 3.3kOhm 1/4W 5% Axial Bulk</t>
+    <t>General Type Carbon Film Resistor 3.3kOhm 1/4W 5% Axial Bulk, General Type Carbon Film Resistor 1kOhm 1/4W 5% Axial Bulk</t>
   </si>
   <si>
     <t>General Type Carbon Film Resistor 220Ohm 1/4W 5% Axial Bulk</t>
@@ -365,6 +365,9 @@
     <t>Arrow Electronics</t>
   </si>
   <si>
+    <t>Rs</t>
+  </si>
+  <si>
     <t>Newark</t>
   </si>
   <si>
@@ -380,9 +383,6 @@
     <t>S7000-ND</t>
   </si>
   <si>
-    <t>26AJ9425</t>
-  </si>
-  <si>
     <t>296-3712-5-ND</t>
   </si>
   <si>
@@ -407,10 +407,10 @@
     <t>D:\continuum\eng\elec\y3s2\ee356\projects\ee356-project\ee356-project\altium_pcb\PCB_Project\PCB_Project.PrjPcb</t>
   </si>
   <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>08 Jan 2023 2158h</t>
+    <t>53</t>
+  </si>
+  <si>
+    <t>08 Feb 2023 1321h</t>
   </si>
   <si>
     <t>Bill of Materials</t>
@@ -2184,11 +2184,11 @@
       </c>
       <c r="D8" s="21">
         <f ca="1">TODAY()</f>
-        <v>44934</v>
+        <v>44965</v>
       </c>
       <c r="E8" s="22">
         <f ca="1">NOW()</f>
-        <v>44934.915892592595</v>
+        <v>44965.556794791664</v>
       </c>
       <c r="F8" s="39"/>
       <c r="G8" s="20"/>
@@ -2228,7 +2228,7 @@
         <v>107</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>122</v>
@@ -2281,10 +2281,10 @@
         <v>2125</v>
       </c>
       <c r="M10" s="85">
-        <v>0.28999999999999998</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="N10" s="85">
-        <v>580</v>
+        <v>450</v>
       </c>
       <c r="O10" s="68" t="s">
         <v>40</v>
@@ -2318,13 +2318,13 @@
         <v>109</v>
       </c>
       <c r="J11" s="32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K11" s="42">
         <v>1000</v>
       </c>
       <c r="L11" s="42">
-        <v>8880</v>
+        <v>0</v>
       </c>
       <c r="M11" s="86">
         <v>1.1440000000000001E-2</v>
@@ -2358,25 +2358,25 @@
         <v>90</v>
       </c>
       <c r="H12" s="30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="77" t="s">
         <v>109</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K12" s="41">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="L12" s="41">
-        <v>8880</v>
+        <v>0</v>
       </c>
       <c r="M12" s="85">
         <v>1.1440000000000001E-2</v>
       </c>
       <c r="N12" s="85">
-        <v>11.44</v>
+        <v>22.88</v>
       </c>
       <c r="O12" s="68" t="s">
         <v>40</v>
@@ -2410,13 +2410,13 @@
         <v>109</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K13" s="42">
         <v>16000</v>
       </c>
       <c r="L13" s="42">
-        <v>8880</v>
+        <v>0</v>
       </c>
       <c r="M13" s="86">
         <v>8.8400000000000006E-3</v>
@@ -2456,7 +2456,7 @@
         <v>110</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K14" s="41">
         <v>4000</v>
@@ -2596,13 +2596,13 @@
         <v>1000</v>
       </c>
       <c r="L17" s="42">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M17" s="86">
-        <v>1.0900000000000001</v>
+        <v>1.01</v>
       </c>
       <c r="N17" s="86">
-        <v>1093.0999999999999</v>
+        <v>1008.17</v>
       </c>
       <c r="O17" s="69" t="s">
         <v>40</v>
@@ -2640,7 +2640,7 @@
         <v>2000</v>
       </c>
       <c r="L18" s="41">
-        <v>66900</v>
+        <v>67296</v>
       </c>
       <c r="M18" s="85">
         <v>0.26205000000000001</v>
@@ -2686,7 +2686,7 @@
         <v>1000</v>
       </c>
       <c r="L19" s="42">
-        <v>932</v>
+        <v>908</v>
       </c>
       <c r="M19" s="86">
         <v>0.13969999999999999</v>
@@ -2724,13 +2724,13 @@
         <v>109</v>
       </c>
       <c r="J20" s="30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K20" s="41">
         <v>1000</v>
       </c>
       <c r="L20" s="41">
-        <v>82887</v>
+        <v>123778</v>
       </c>
       <c r="M20" s="85">
         <v>0.15278</v>
@@ -2807,10 +2807,10 @@
         <v>1</v>
       </c>
       <c r="I23" s="78" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="J23" s="32">
-        <v>1715487</v>
+        <v>1310276</v>
       </c>
       <c r="K23" s="42">
         <v>1000</v>
@@ -2819,10 +2819,10 @@
         <v>0</v>
       </c>
       <c r="M23" s="86">
-        <v>3.24</v>
+        <v>2.75</v>
       </c>
       <c r="N23" s="86">
-        <v>3239.26</v>
+        <v>2753.98</v>
       </c>
       <c r="O23" s="69" t="s">
         <v>40</v>
@@ -2851,20 +2851,20 @@
       <c r="I24" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="J24" s="30" t="s">
-        <v>119</v>
+      <c r="J24" s="30">
+        <v>1000763</v>
       </c>
       <c r="K24" s="41">
         <v>1000</v>
       </c>
       <c r="L24" s="41">
-        <v>0</v>
+        <v>3750</v>
       </c>
       <c r="M24" s="85">
-        <v>0.64200000000000002</v>
+        <v>0.45617000000000002</v>
       </c>
       <c r="N24" s="85">
-        <v>642</v>
+        <v>456.17</v>
       </c>
       <c r="O24" s="68" t="s">
         <v>40</v>
@@ -2900,7 +2900,7 @@
         <v>2000</v>
       </c>
       <c r="L25" s="42">
-        <v>6198</v>
+        <v>5948</v>
       </c>
       <c r="M25" s="86">
         <v>0.82076000000000005</v>
@@ -2947,10 +2947,10 @@
         <v>0</v>
       </c>
       <c r="M26" s="85">
-        <v>0.44500000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="N26" s="85">
-        <v>890</v>
+        <v>720</v>
       </c>
       <c r="O26" s="68" t="s">
         <v>40</v>
@@ -2974,7 +2974,7 @@
         <v>103</v>
       </c>
       <c r="H27" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I27" s="78" t="s">
         <v>111</v>
@@ -2983,16 +2983,16 @@
         <v>2938971</v>
       </c>
       <c r="K27" s="42">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="L27" s="42">
         <v>0</v>
       </c>
       <c r="M27" s="86">
-        <v>0.12981000000000001</v>
+        <v>0.14194999999999999</v>
       </c>
       <c r="N27" s="86">
-        <v>259.63</v>
+        <v>425.84</v>
       </c>
       <c r="O27" s="69" t="s">
         <v>40</v>
@@ -3051,7 +3051,7 @@
         <v>3</v>
       </c>
       <c r="I29" s="78" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J29" s="32" t="s">
         <v>121</v>
@@ -3060,13 +3060,13 @@
         <v>3000</v>
       </c>
       <c r="L29" s="42">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M29" s="86">
-        <v>0.71599999999999997</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="N29" s="86">
-        <v>2148</v>
+        <v>2058</v>
       </c>
       <c r="O29" s="69" t="s">
         <v>40</v>
@@ -3082,19 +3082,19 @@
       <c r="G30" s="39"/>
       <c r="H30" s="48">
         <f>SUM(H10:H29)</f>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I30" s="79"/>
       <c r="J30" s="43"/>
       <c r="K30" s="48">
         <f>SUM(K10:K29)</f>
-        <v>43000</v>
+        <v>45000</v>
       </c>
       <c r="L30" s="47"/>
       <c r="M30" s="47"/>
       <c r="N30" s="47">
         <f>SUM(N10:N29)</f>
-        <v>19156.290000000005</v>
+        <v>18187.900000000001</v>
       </c>
       <c r="O30" s="70"/>
     </row>
@@ -3139,7 +3139,7 @@
       <c r="K32" s="39"/>
       <c r="L32" s="88">
         <f>N30</f>
-        <v>19156.290000000005</v>
+        <v>18187.900000000001</v>
       </c>
       <c r="M32" s="89"/>
       <c r="N32" s="97" t="s">
@@ -3163,7 +3163,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="90">
         <f>L32/H32</f>
-        <v>19.156290000000006</v>
+        <v>18.187900000000003</v>
       </c>
       <c r="M33" s="90"/>
       <c r="N33" s="98" t="s">

</xml_diff>